<commit_message>
Amélioration de résultats pour deux phrases
Ajouter des données manquantes des l'excel.
</commit_message>
<xml_diff>
--- a/Fichier_Dictionnaire.xlsx
+++ b/Fichier_Dictionnaire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\Projet Terminator\1003\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Idriss\Downloads\Terminator-master\Terminator-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FAB77C-C320-48E0-8080-D8BBDD47267B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0837622E-750F-4D65-9F2E-305A13BAF519}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organes" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2318" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="1047">
   <si>
     <t>Property</t>
   </si>
@@ -3162,6 +3162,9 @@
   </si>
   <si>
     <t>not visible</t>
+  </si>
+  <si>
+    <t>curved dorsally</t>
   </si>
 </sst>
 </file>
@@ -4401,10 +4404,10 @@
       <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="74" style="1" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -42130,16 +42133,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C153"/>
+  <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -42439,7 +42442,7 @@
       </c>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" ht="22.5">
+    <row r="34" spans="1:3">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -42583,7 +42586,7 @@
       </c>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="1:3" ht="22.5">
+    <row r="50" spans="1:3">
       <c r="A50" s="3" t="s">
         <v>53</v>
       </c>
@@ -42601,7 +42604,7 @@
       </c>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:3" ht="22.5">
+    <row r="52" spans="1:3">
       <c r="A52" s="3" t="s">
         <v>53</v>
       </c>
@@ -42619,7 +42622,7 @@
       </c>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="1:3" ht="22.5">
+    <row r="54" spans="1:3">
       <c r="A54" s="3" t="s">
         <v>52</v>
       </c>
@@ -42628,7 +42631,7 @@
       </c>
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="1:3" ht="22.5">
+    <row r="55" spans="1:3">
       <c r="A55" s="3" t="s">
         <v>52</v>
       </c>
@@ -42828,19 +42831,19 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>468</v>
+        <v>771</v>
       </c>
       <c r="C77" s="3"/>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>476</v>
+        <v>600</v>
       </c>
       <c r="C78" s="3"/>
     </row>
@@ -42849,16 +42852,16 @@
         <v>51</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>701</v>
+        <v>468</v>
       </c>
       <c r="C79" s="3"/>
     </row>
-    <row r="80" spans="1:3" ht="22.5">
+    <row r="80" spans="1:3">
       <c r="A80" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>610</v>
+        <v>476</v>
       </c>
       <c r="C80" s="3"/>
     </row>
@@ -42867,16 +42870,16 @@
         <v>51</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>591</v>
+        <v>701</v>
       </c>
       <c r="C81" s="3"/>
     </row>
-    <row r="82" spans="1:3" ht="22.5">
+    <row r="82" spans="1:3">
       <c r="A82" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>592</v>
+        <v>610</v>
       </c>
       <c r="C82" s="3"/>
     </row>
@@ -42885,25 +42888,25 @@
         <v>51</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>727</v>
+        <v>591</v>
       </c>
       <c r="C83" s="3"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="3" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C84" s="3"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="3" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>59</v>
+        <v>727</v>
       </c>
       <c r="C85" s="3"/>
     </row>
@@ -42912,25 +42915,25 @@
         <v>39</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>62</v>
+        <v>593</v>
       </c>
       <c r="C86" s="3"/>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>496</v>
+        <v>59</v>
       </c>
       <c r="C87" s="3"/>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>594</v>
+        <v>62</v>
       </c>
       <c r="C88" s="3"/>
     </row>
@@ -42939,25 +42942,25 @@
         <v>52</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>595</v>
+        <v>496</v>
       </c>
       <c r="C89" s="3"/>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C90" s="3"/>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>619</v>
+        <v>595</v>
       </c>
       <c r="C91" s="3"/>
     </row>
@@ -42966,7 +42969,7 @@
         <v>48</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>757</v>
+        <v>596</v>
       </c>
       <c r="C92" s="3"/>
     </row>
@@ -42975,7 +42978,7 @@
         <v>48</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C93" s="3"/>
     </row>
@@ -42984,7 +42987,7 @@
         <v>48</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>842</v>
+        <v>757</v>
       </c>
       <c r="C94" s="3"/>
     </row>
@@ -42993,7 +42996,7 @@
         <v>48</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>758</v>
+        <v>620</v>
       </c>
       <c r="C95" s="3"/>
     </row>
@@ -43002,7 +43005,7 @@
         <v>48</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>669</v>
+        <v>842</v>
       </c>
       <c r="C96" s="3"/>
     </row>
@@ -43011,7 +43014,7 @@
         <v>48</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>553</v>
+        <v>758</v>
       </c>
       <c r="C97" s="3"/>
     </row>
@@ -43020,7 +43023,7 @@
         <v>48</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>729</v>
+        <v>669</v>
       </c>
       <c r="C98" s="3"/>
     </row>
@@ -43029,7 +43032,7 @@
         <v>48</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>621</v>
+        <v>553</v>
       </c>
       <c r="C99" s="3"/>
     </row>
@@ -43038,7 +43041,7 @@
         <v>48</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>599</v>
+        <v>729</v>
       </c>
       <c r="C100" s="3"/>
     </row>
@@ -43047,25 +43050,25 @@
         <v>48</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>600</v>
+        <v>621</v>
       </c>
       <c r="C101" s="3"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="3" t="s">
-        <v>575</v>
+        <v>48</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>719</v>
+        <v>599</v>
       </c>
       <c r="C102" s="3"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="3" t="s">
-        <v>575</v>
+        <v>48</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>720</v>
+        <v>600</v>
       </c>
       <c r="C103" s="3"/>
     </row>
@@ -43074,7 +43077,7 @@
         <v>575</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C104" s="3"/>
     </row>
@@ -43083,7 +43086,7 @@
         <v>575</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>736</v>
+        <v>720</v>
       </c>
       <c r="C105" s="3"/>
     </row>
@@ -43092,7 +43095,7 @@
         <v>575</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C106" s="3"/>
     </row>
@@ -43101,7 +43104,7 @@
         <v>575</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>723</v>
+        <v>736</v>
       </c>
       <c r="C107" s="3"/>
     </row>
@@ -43110,34 +43113,34 @@
         <v>575</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>828</v>
+        <v>722</v>
       </c>
       <c r="C108" s="3"/>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="3" t="s">
-        <v>760</v>
+        <v>575</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>761</v>
+        <v>723</v>
       </c>
       <c r="C109" s="3"/>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="3" t="s">
-        <v>760</v>
+        <v>575</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>762</v>
+        <v>1046</v>
       </c>
       <c r="C110" s="3"/>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="3" t="s">
-        <v>760</v>
+        <v>575</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>763</v>
+        <v>828</v>
       </c>
       <c r="C111" s="3"/>
     </row>
@@ -43146,7 +43149,7 @@
         <v>760</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="C112" s="3"/>
     </row>
@@ -43155,7 +43158,7 @@
         <v>760</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="C113" s="3"/>
     </row>
@@ -43164,7 +43167,7 @@
         <v>760</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="C114" s="3"/>
     </row>
@@ -43173,7 +43176,7 @@
         <v>760</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="C115" s="3"/>
     </row>
@@ -43182,7 +43185,7 @@
         <v>760</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="C116" s="3"/>
     </row>
@@ -43191,7 +43194,7 @@
         <v>760</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="C117" s="3"/>
     </row>
@@ -43200,30 +43203,45 @@
         <v>760</v>
       </c>
       <c r="B118" s="3" t="s">
+        <v>767</v>
+      </c>
+      <c r="C118" s="3"/>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="C119" s="3"/>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>769</v>
+      </c>
+      <c r="C120" s="3"/>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="B121" s="3" t="s">
         <v>770</v>
       </c>
-      <c r="C118" s="3"/>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="C119" s="3"/>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="C120" s="3"/>
-    </row>
-    <row r="121" spans="1:3">
       <c r="C121" s="3"/>
     </row>
-    <row r="145" spans="1:2">
-      <c r="A145" s="3"/>
-      <c r="B145" s="3"/>
-    </row>
-    <row r="146" spans="1:2">
-      <c r="A146" s="3"/>
-      <c r="B146" s="3"/>
-    </row>
-    <row r="147" spans="1:2">
-      <c r="A147" s="3"/>
-      <c r="B147" s="3"/>
+    <row r="122" spans="1:3">
+      <c r="C122" s="3"/>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="C123" s="3"/>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="C124" s="3"/>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="3"/>
@@ -43243,9 +43261,21 @@
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="3"/>
+      <c r="B152" s="3"/>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="3"/>
+      <c r="B153" s="3"/>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="3"/>
+      <c r="B154" s="3"/>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="3"/>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43260,13 +43290,13 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.26953125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="25.5">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1026</v>
       </c>
@@ -43274,7 +43304,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="25.5">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1026</v>
       </c>
@@ -43282,7 +43312,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="25.5">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>1026</v>
       </c>
@@ -43290,7 +43320,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="25.5">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>1026</v>
       </c>
@@ -43298,7 +43328,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="25.5">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>1026</v>
       </c>
@@ -43306,7 +43336,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="25.5">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>1027</v>
       </c>
@@ -43314,7 +43344,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="25.5">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>1027</v>
       </c>
@@ -43322,7 +43352,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="25.5">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>1027</v>
       </c>
@@ -43330,7 +43360,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="25.5">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>1027</v>
       </c>
@@ -43338,7 +43368,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="25.5">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>1027</v>
       </c>
@@ -43346,7 +43376,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="25.5">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>1027</v>
       </c>
@@ -43354,7 +43384,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="25.5">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>1027</v>
       </c>
@@ -43362,7 +43392,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="25.5">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>1027</v>
       </c>
@@ -43481,13 +43511,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67029488-FF29-4A4F-8776-A962EBE7AA7E}">
-  <dimension ref="A1:B187"/>
+  <dimension ref="A1:B186"/>
   <sheetViews>
     <sheetView topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="D174" sqref="D174"/>
+      <selection activeCell="A159" sqref="A159:XFD159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
@@ -43723,7 +43753,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="22.5">
+    <row r="36" spans="1:2">
       <c r="A36" s="3" t="s">
         <v>12</v>
       </c>
@@ -43819,7 +43849,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="22.5">
+    <row r="48" spans="1:2" ht="21">
       <c r="A48" s="3" t="s">
         <v>15</v>
       </c>
@@ -44033,7 +44063,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="22.5">
+    <row r="76" spans="1:2">
       <c r="A76" s="3" t="s">
         <v>58</v>
       </c>
@@ -44041,7 +44071,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="22.5">
+    <row r="77" spans="1:2">
       <c r="A77" s="3" t="s">
         <v>58</v>
       </c>
@@ -44049,7 +44079,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="22.5">
+    <row r="78" spans="1:2">
       <c r="A78" s="3" t="s">
         <v>58</v>
       </c>
@@ -44135,7 +44165,7 @@
       </c>
       <c r="B91" s="3"/>
     </row>
-    <row r="92" spans="1:2" ht="22.5">
+    <row r="92" spans="1:2" ht="21">
       <c r="A92" s="3" t="s">
         <v>482</v>
       </c>
@@ -44143,7 +44173,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="22.5">
+    <row r="93" spans="1:2" ht="21">
       <c r="A93" s="3" t="s">
         <v>482</v>
       </c>
@@ -44159,7 +44189,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="22.5">
+    <row r="95" spans="1:2">
       <c r="A95" s="3" t="s">
         <v>486</v>
       </c>
@@ -44177,7 +44207,7 @@
       </c>
       <c r="B97" s="3"/>
     </row>
-    <row r="98" spans="1:2" ht="22.5">
+    <row r="98" spans="1:2">
       <c r="A98" s="3" t="s">
         <v>500</v>
       </c>
@@ -44345,7 +44375,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="22.5">
+    <row r="123" spans="1:2">
       <c r="A123" s="3" t="s">
         <v>1031</v>
       </c>
@@ -44363,7 +44393,7 @@
       </c>
       <c r="B125" s="3"/>
     </row>
-    <row r="126" spans="1:2" ht="22.5">
+    <row r="126" spans="1:2">
       <c r="A126" s="3" t="s">
         <v>1034</v>
       </c>
@@ -44437,7 +44467,7 @@
       </c>
       <c r="B136" s="3"/>
     </row>
-    <row r="137" spans="1:2" ht="22.5">
+    <row r="137" spans="1:2">
       <c r="A137" s="3" t="s">
         <v>610</v>
       </c>
@@ -44449,7 +44479,7 @@
       </c>
       <c r="B138" s="3"/>
     </row>
-    <row r="139" spans="1:2" ht="22.5">
+    <row r="139" spans="1:2">
       <c r="A139" s="3" t="s">
         <v>592</v>
       </c>
@@ -44585,34 +44615,36 @@
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="3" t="s">
-        <v>600</v>
+        <v>636</v>
       </c>
       <c r="B159" s="3"/>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="3" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B160" s="3"/>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="3" t="s">
-        <v>637</v>
+        <v>869</v>
       </c>
       <c r="B161" s="3"/>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="3" t="s">
-        <v>869</v>
-      </c>
-      <c r="B162" s="3"/>
+        <v>639</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>638</v>
+      </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="3" t="s">
         <v>639</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -44620,145 +44652,137 @@
         <v>639</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>640</v>
+        <v>868</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="3" t="s">
-        <v>639</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>868</v>
-      </c>
+        <v>1036</v>
+      </c>
+      <c r="B165" s="3"/>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="3" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="B166" s="3"/>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="3" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="B167" s="3"/>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="3" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B168" s="3"/>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="3" t="s">
-        <v>1039</v>
+        <v>663</v>
       </c>
       <c r="B169" s="3"/>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="3" t="s">
-        <v>663</v>
+        <v>719</v>
       </c>
       <c r="B170" s="3"/>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="3" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B171" s="3"/>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="3" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B172" s="3"/>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="3" t="s">
-        <v>721</v>
+        <v>736</v>
       </c>
       <c r="B173" s="3"/>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="3" t="s">
-        <v>736</v>
+        <v>722</v>
       </c>
       <c r="B174" s="3"/>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="3" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B175" s="3"/>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="3" t="s">
-        <v>723</v>
+        <v>828</v>
       </c>
       <c r="B176" s="3"/>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" s="3" t="s">
-        <v>828</v>
+        <v>761</v>
       </c>
       <c r="B177" s="3"/>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="3" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B178" s="3"/>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" s="3" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B179" s="3"/>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="3" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B180" s="3"/>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="3" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B181" s="3"/>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="3" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B182" s="3"/>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="3" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B183" s="3"/>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="3" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B184" s="3"/>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="3" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B185" s="3"/>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="3" t="s">
-        <v>769</v>
-      </c>
-      <c r="B186" s="3"/>
-    </row>
-    <row r="187" spans="1:2">
-      <c r="A187" s="3" t="s">
         <v>770</v>
       </c>
     </row>
@@ -44775,15 +44799,15 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="62.140625" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
-    <col min="4" max="4" width="58.140625" customWidth="1"/>
+    <col min="1" max="1" width="62.1796875" customWidth="1"/>
+    <col min="2" max="2" width="35.1796875" customWidth="1"/>
+    <col min="3" max="3" width="31.7265625" customWidth="1"/>
+    <col min="4" max="4" width="58.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" ht="14">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -46073,7 +46097,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="22.5">
+    <row r="101" spans="1:4" ht="21">
       <c r="A101" s="3" t="s">
         <v>156</v>
       </c>
@@ -46183,7 +46207,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="22.5">
+    <row r="110" spans="1:4">
       <c r="A110" s="3" t="s">
         <v>165</v>
       </c>
@@ -46195,7 +46219,7 @@
       </c>
       <c r="D110" s="3"/>
     </row>
-    <row r="111" spans="1:4" ht="22.5">
+    <row r="111" spans="1:4" ht="21">
       <c r="A111" s="3" t="s">
         <v>165</v>
       </c>

</xml_diff>